<commit_message>
update excel tool builder
</commit_message>
<xml_diff>
--- a/My_application/third_party/PHPExcel/finance/test5.xlsx
+++ b/My_application/third_party/PHPExcel/finance/test5.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genny\Desktop\Mind Cloud Tribe\Videos\Videos 11_13_14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cloud\My_application\third_party\PHPExcel\finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8123D52-06CB-4FD2-BB47-56112E857FC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10455"/>
   </bookViews>
   <sheets>
     <sheet name="Break-Even Point" sheetId="1" r:id="rId1"/>
@@ -25,9 +24,6 @@
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -128,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -473,7 +469,7 @@
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -774,7 +770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
@@ -782,23 +778,22 @@
   <dimension ref="B1:I42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="8" width="3.453125" customWidth="1"/>
-    <col min="9" max="9" width="102.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="8" width="3.42578125" customWidth="1"/>
+    <col min="9" max="9" width="102.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
@@ -810,7 +805,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="44" t="s">
@@ -821,7 +816,7 @@
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45"/>
       <c r="C3" s="16"/>
       <c r="D3" s="44" t="s">
@@ -833,7 +828,7 @@
       </c>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="43"/>
       <c r="C4" s="16"/>
       <c r="D4" s="44" t="s">
@@ -845,14 +840,14 @@
       </c>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="2:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
         <v>22</v>
       </c>
@@ -861,7 +856,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="37"/>
       <c r="C7" s="51" t="s">
         <v>0</v>
@@ -872,7 +867,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="37"/>
       <c r="C8" s="49" t="s">
         <v>1</v>
@@ -881,7 +876,7 @@
       <c r="E8" s="49"/>
       <c r="F8" s="23"/>
     </row>
-    <row r="9" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="37"/>
       <c r="C9" s="49" t="s">
         <v>2</v>
@@ -890,7 +885,7 @@
       <c r="E9" s="49"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="37"/>
       <c r="C10" s="49" t="s">
         <v>3</v>
@@ -899,7 +894,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="37"/>
       <c r="C11" s="49" t="s">
         <v>4</v>
@@ -910,7 +905,7 @@
         <v>149000</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="37"/>
       <c r="C12" s="49" t="s">
         <v>5</v>
@@ -921,7 +916,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="37"/>
       <c r="C13" s="49" t="s">
         <v>10</v>
@@ -930,7 +925,7 @@
       <c r="E13" s="49"/>
       <c r="F13" s="23"/>
     </row>
-    <row r="14" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="37"/>
       <c r="C14" s="49" t="s">
         <v>10</v>
@@ -939,7 +934,7 @@
       <c r="E14" s="49"/>
       <c r="F14" s="23"/>
     </row>
-    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="38"/>
       <c r="C15" s="50" t="s">
         <v>10</v>
@@ -948,7 +943,7 @@
       <c r="E15" s="50"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="39" t="s">
         <v>6</v>
       </c>
@@ -960,14 +955,14 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="36" t="s">
         <v>23</v>
       </c>
@@ -976,7 +971,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="39" t="s">
         <v>15</v>
       </c>
@@ -985,7 +980,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="37"/>
       <c r="C20" s="20" t="s">
         <v>7</v>
@@ -998,7 +993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="37"/>
       <c r="C21" s="22" t="s">
         <v>8</v>
@@ -1009,7 +1004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="37"/>
       <c r="C22" s="22" t="s">
         <v>9</v>
@@ -1020,7 +1015,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="37"/>
       <c r="C23" s="24" t="s">
         <v>25</v>
@@ -1031,7 +1026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="37"/>
       <c r="C24" s="18"/>
       <c r="D24" s="26" t="s">
@@ -1043,14 +1038,14 @@
       </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="2:6" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="39" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1057,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
       <c r="C27" s="27" t="s">
         <v>20</v>
@@ -1074,7 +1069,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="27" t="s">
         <v>21</v>
@@ -1086,14 +1081,14 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="40"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="41" t="s">
         <v>24</v>
       </c>
@@ -1102,7 +1097,7 @@
       <c r="E30" s="31"/>
       <c r="F30" s="32"/>
     </row>
-    <row r="31" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="42" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1111,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="42" t="s">
         <v>14</v>
       </c>
@@ -1130,32 +1125,32 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B33" s="9"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
     </row>
   </sheetData>

</xml_diff>